<commit_message>
Code Updated - Version 1
</commit_message>
<xml_diff>
--- a/excelFiles/testExcel.xlsx
+++ b/excelFiles/testExcel.xlsx
@@ -1,35 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jenkins\workspace\Jenkins Report Generator\excelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+  <si>
+    <t>Job Name</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Overall Status</t>
+  </si>
+  <si>
+    <t>Feature File Count</t>
+  </si>
+  <si>
+    <t>DAM Custom Execution</t>
+  </si>
+  <si>
+    <t>00:01:09.305</t>
+  </si>
+  <si>
+    <t>00:01:29.283</t>
+  </si>
+  <si>
+    <t>00:01:06.057</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>00:01:06.897</t>
+  </si>
+  <si>
+    <t>00:01:23.227</t>
+  </si>
+  <si>
+    <t>00:01:08.639</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,81 +100,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -411,115 +411,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Job Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Duration</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>DAM Custom Execution</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30 seconds</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DAM Custom Execution</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>30 seconds</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DAM Custom Execution</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>30 seconds</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>DAM Custom Execution</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>30 seconds</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>